<commit_message>
Map settings menu layout
</commit_message>
<xml_diff>
--- a/Worms/Worms/Textures/MapSettingsMenu/MapSettings.xlsx
+++ b/Worms/Worms/Textures/MapSettingsMenu/MapSettings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\Worms-SFML\Worms\Worms\Textures\NewGameMenu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\Worms-SFML\Worms\Worms\Textures\MapSettingsMenu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B3ACAD-CA82-4987-84DD-2B0A4FBBE79E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2A6EFE-8721-459C-9596-246860C51290}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="3675" xr2:uid="{265BE817-B86D-4E0D-985A-801E2BE0A218}"/>
   </bookViews>
@@ -25,19 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>Map Set</t>
-  </si>
-  <si>
-    <t>Game Set</t>
-  </si>
-  <si>
-    <t>Weap Set</t>
-  </si>
-  <si>
-    <t>Team Set</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t xml:space="preserve">Worm </t>
   </si>
@@ -63,10 +51,28 @@
     <t>Load Conf</t>
   </si>
   <si>
-    <t>Start</t>
-  </si>
-  <si>
     <t>Back</t>
+  </si>
+  <si>
+    <t>PenWidth</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Tunels count</t>
+  </si>
+  <si>
+    <t>Spheres count</t>
+  </si>
+  <si>
+    <t>reverse map</t>
+  </si>
+  <si>
+    <t>tunels</t>
+  </si>
+  <si>
+    <t>spheres</t>
   </si>
 </sst>
 </file>
@@ -83,12 +89,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -103,8 +115,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -421,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2A68B7-6894-47E5-8E48-DC2A8B28DF90}">
   <dimension ref="E4:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N13" workbookViewId="0">
-      <selection activeCell="AW14" sqref="AW14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,6 +483,17 @@
       <c r="E5">
         <v>1</v>
       </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
       <c r="Q5">
         <v>1</v>
       </c>
@@ -478,6 +502,17 @@
       <c r="E6">
         <v>2</v>
       </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
       <c r="Q6">
         <v>2</v>
       </c>
@@ -486,6 +521,17 @@
       <c r="E7">
         <v>3</v>
       </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
       <c r="Q7">
         <v>3</v>
       </c>
@@ -494,15 +540,17 @@
       <c r="E8">
         <v>4</v>
       </c>
-      <c r="H8" t="s">
-        <v>0</v>
-      </c>
-      <c r="K8" t="s">
-        <v>10</v>
-      </c>
-      <c r="N8" t="s">
-        <v>2</v>
-      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
       <c r="Q8">
         <v>4</v>
       </c>
@@ -511,6 +559,17 @@
       <c r="E9">
         <v>5</v>
       </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
       <c r="Q9">
         <v>5</v>
       </c>
@@ -519,15 +578,17 @@
       <c r="E10">
         <v>6</v>
       </c>
-      <c r="H10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K10" t="s">
-        <v>11</v>
-      </c>
-      <c r="N10" t="s">
-        <v>3</v>
-      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
       <c r="Q10">
         <v>6</v>
       </c>
@@ -536,6 +597,17 @@
       <c r="E11">
         <v>7</v>
       </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
       <c r="Q11">
         <v>7</v>
       </c>
@@ -544,6 +616,17 @@
       <c r="E12">
         <v>8</v>
       </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
       <c r="Q12">
         <v>8</v>
       </c>
@@ -560,6 +643,15 @@
       <c r="E14">
         <v>10</v>
       </c>
+      <c r="H14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" t="s">
+        <v>13</v>
+      </c>
       <c r="Q14">
         <v>10</v>
       </c>
@@ -576,17 +668,17 @@
       <c r="E16">
         <v>12</v>
       </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>2</v>
-      </c>
-      <c r="L16">
-        <v>3</v>
-      </c>
-      <c r="N16">
-        <v>4</v>
+      <c r="H16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16" t="s">
+        <v>6</v>
       </c>
       <c r="Q16">
         <v>12</v>
@@ -605,10 +697,19 @@
         <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
-      </c>
-      <c r="P18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" t="s">
         <v>12</v>
+      </c>
+      <c r="I18" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" t="s">
+        <v>15</v>
+      </c>
+      <c r="O18" t="s">
+        <v>7</v>
       </c>
       <c r="Q18">
         <v>14</v>
@@ -662,10 +763,10 @@
         <v>4</v>
       </c>
       <c r="G23" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="5:17" x14ac:dyDescent="0.25">
@@ -673,7 +774,7 @@
         <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="5:17" x14ac:dyDescent="0.25">
@@ -681,10 +782,10 @@
         <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H25" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="5:17" x14ac:dyDescent="0.25">
@@ -692,10 +793,10 @@
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H26" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>